<commit_message>
adding supplementary tables 3 and 4
</commit_message>
<xml_diff>
--- a/manuscript/Figures_&_tables/Supplementary Table 3 ANOVAs.xlsx
+++ b/manuscript/Figures_&_tables/Supplementary Table 3 ANOVAs.xlsx
@@ -969,7 +969,7 @@
   <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,8 +978,9 @@
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update all figures from root surf to root area
</commit_message>
<xml_diff>
--- a/manuscript/Figures_&_tables/Supplementary Table 3 ANOVAs.xlsx
+++ b/manuscript/Figures_&_tables/Supplementary Table 3 ANOVAs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\montazeaud\Documents\RECHERCHE\Postdoc\Montpellier\SolACE 3\SolACE_wheat_mixtures\manuscript\Figures_&amp;_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC97182-0373-491C-97E1-140E02BC58F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -578,9 +579,6 @@
     <t>0.339435057192555</t>
   </si>
   <si>
-    <t>Root surface (mm²)</t>
-  </si>
-  <si>
     <t>910974928.194203</t>
   </si>
   <si>
@@ -630,12 +628,15 @@
   </si>
   <si>
     <t>0.402056737603252</t>
+  </si>
+  <si>
+    <t>Root projected area (mm²)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -965,11 +966,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2088,7 +2089,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2116,22 +2117,22 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
+        <v>184</v>
+      </c>
+      <c r="C69" t="s">
         <v>185</v>
-      </c>
-      <c r="C69" t="s">
-        <v>186</v>
       </c>
       <c r="D69">
         <v>2</v>
       </c>
       <c r="E69" t="s">
+        <v>186</v>
+      </c>
+      <c r="F69" t="s">
         <v>187</v>
       </c>
-      <c r="F69" t="s">
+      <c r="G69" t="s">
         <v>188</v>
-      </c>
-      <c r="G69" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2139,22 +2140,22 @@
         <v>17</v>
       </c>
       <c r="B70" t="s">
+        <v>189</v>
+      </c>
+      <c r="C70" t="s">
+        <v>189</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
         <v>190</v>
       </c>
-      <c r="C70" t="s">
-        <v>190</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-      <c r="E70" t="s">
+      <c r="F70" t="s">
         <v>191</v>
       </c>
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>192</v>
-      </c>
-      <c r="G70" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2162,22 +2163,22 @@
         <v>22</v>
       </c>
       <c r="B71" t="s">
+        <v>193</v>
+      </c>
+      <c r="C71" t="s">
+        <v>193</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
         <v>194</v>
       </c>
-      <c r="C71" t="s">
-        <v>194</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>195</v>
       </c>
-      <c r="F71" t="s">
+      <c r="G71" t="s">
         <v>196</v>
-      </c>
-      <c r="G71" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2185,22 +2186,22 @@
         <v>27</v>
       </c>
       <c r="B72" t="s">
+        <v>197</v>
+      </c>
+      <c r="C72" t="s">
+        <v>197</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72" t="s">
         <v>198</v>
       </c>
-      <c r="C72" t="s">
-        <v>198</v>
-      </c>
-      <c r="D72">
-        <v>1</v>
-      </c>
-      <c r="E72" t="s">
+      <c r="F72" t="s">
         <v>199</v>
       </c>
-      <c r="F72" t="s">
+      <c r="G72" t="s">
         <v>200</v>
-      </c>
-      <c r="G72" t="s">
-        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>